<commit_message>
Code & Data OK
</commit_message>
<xml_diff>
--- a/leretour/manuel/vocabulaire.xlsx
+++ b/leretour/manuel/vocabulaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoine/Documents/antoine/apple iigs/crossdevtools/source/leretour/manuel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2367A48A-2635-424C-B9C7-F2DF159DE23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A12044F-5732-0C48-A6BF-330C7B971CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{0E21123E-A662-2741-A5F5-03AB1B6E5065}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="247">
   <si>
     <t>FR</t>
   </si>
@@ -773,6 +773,9 @@
   </si>
   <si>
     <t>WITH</t>
+  </si>
+  <si>
+    <t>BLUE</t>
   </si>
 </sst>
 </file>
@@ -1126,8 +1129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51DC3DE-58FF-F645-A0E2-B8E802529A8C}">
   <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C142"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1421,7 +1424,7 @@
         <v>36</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>